<commit_message>
updated TODO for P_leaching risk_comb
</commit_message>
<xml_diff>
--- a/27087_attachments/synthesis_grassland_function_metadata_ID27087.xlsx
+++ b/27087_attachments/synthesis_grassland_function_metadata_ID27087.xlsx
@@ -12,8 +12,8 @@
     <sheet name="description_of_columns" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">synthesis_grassland_function_me!$A$1:$X$91</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">synthesis_grassland_function_me!$A$1:$X$89</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">synthesis_grassland_function_me!$A$1:$X$89</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">synthesis_grassland_function_me!$A$1:$X$91</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1609" uniqueCount="705">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1609" uniqueCount="704">
   <si>
     <t xml:space="preserve">ColumnName</t>
   </si>
@@ -1926,9 +1926,6 @@
 variable used to assemble PRI</t>
   </si>
   <si>
-    <t xml:space="preserve">P_leaching_risk_comb rename to Phosphorous_hold or Phosphorous_holdback</t>
-  </si>
-  <si>
     <t xml:space="preserve">P_leaching_risk_comb</t>
   </si>
   <si>
@@ -1981,7 +1978,8 @@
 if one value was missing, the value of the present year was taken</t>
   </si>
   <si>
-    <t xml:space="preserve">very similar to PRI, do not include both to the same analysis</t>
+    <t xml:space="preserve">very similar to PRI, do not include both to the same analysis
+TODO  rename to Phosphorous_hold or Phosphorous_holdback</t>
   </si>
   <si>
     <t xml:space="preserve">P_leaching_risk</t>
@@ -3578,11 +3576,11 @@
   <dimension ref="A1:Y91"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="V53" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topRight" activeCell="V1" activeCellId="0" sqref="V1"/>
+      <selection pane="bottomLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
+      <selection pane="bottomRight" activeCell="X58" activeCellId="0" sqref="X58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="36" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7701,7 +7699,7 @@
         <v>414</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C57" s="1" t="n">
         <v>444444</v>
@@ -7710,7 +7708,7 @@
         <v>150</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G57" s="1" t="n">
         <v>1</v>
@@ -7722,10 +7720,10 @@
         <v>88</v>
       </c>
       <c r="Q57" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="R57" s="5" t="s">
         <v>417</v>
-      </c>
-      <c r="R57" s="5" t="s">
-        <v>418</v>
       </c>
       <c r="S57" s="1" t="s">
         <v>34</v>
@@ -7734,16 +7732,16 @@
         <v>313</v>
       </c>
       <c r="U57" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="V57" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="V57" s="1" t="s">
+      <c r="W57" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="W57" s="1" t="s">
+      <c r="X57" s="1" t="s">
         <v>421</v>
-      </c>
-      <c r="X57" s="1" t="s">
-        <v>422</v>
       </c>
       <c r="Y57" s="1" t="s">
         <v>40</v>
@@ -7751,16 +7749,16 @@
     </row>
     <row r="58" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="12" t="s">
+        <v>422</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>423</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>424</v>
       </c>
       <c r="C58" s="1" t="n">
         <v>2015</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E58" s="1" t="n">
         <v>148</v>
@@ -7775,49 +7773,49 @@
         <v>20447</v>
       </c>
       <c r="I58" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="J58" s="1" t="s">
         <v>425</v>
-      </c>
-      <c r="J58" s="1" t="s">
-        <v>426</v>
       </c>
       <c r="K58" s="1" t="n">
         <v>2</v>
       </c>
       <c r="L58" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="M58" s="1" t="s">
         <v>307</v>
       </c>
       <c r="N58" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="O58" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="P58" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="O58" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="P58" s="1" t="s">
+      <c r="Q58" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="Q58" s="1" t="s">
+      <c r="R58" s="5" t="s">
         <v>430</v>
-      </c>
-      <c r="R58" s="5" t="s">
-        <v>431</v>
       </c>
       <c r="S58" s="1" t="s">
         <v>34</v>
       </c>
       <c r="T58" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="U58" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="V58" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="U58" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="V58" s="1" t="s">
+      <c r="W58" s="1" t="s">
         <v>433</v>
-      </c>
-      <c r="W58" s="1" t="s">
-        <v>434</v>
       </c>
       <c r="Y58" s="1" t="s">
         <v>40</v>
@@ -7825,16 +7823,16 @@
     </row>
     <row r="59" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="12" t="s">
+        <v>434</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>435</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>436</v>
       </c>
       <c r="C59" s="1" t="n">
         <v>2011</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E59" s="1" t="n">
         <v>150</v>
@@ -7849,16 +7847,16 @@
         <v>19009</v>
       </c>
       <c r="I59" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="J59" s="1" t="s">
         <v>437</v>
-      </c>
-      <c r="J59" s="1" t="s">
-        <v>438</v>
       </c>
       <c r="K59" s="1" t="n">
         <v>2</v>
       </c>
       <c r="L59" s="6" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="M59" s="1" t="s">
         <v>324</v>
@@ -7873,25 +7871,25 @@
         <v>410</v>
       </c>
       <c r="Q59" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="R59" s="5" t="s">
         <v>440</v>
-      </c>
-      <c r="R59" s="5" t="s">
-        <v>441</v>
       </c>
       <c r="S59" s="1" t="s">
         <v>34</v>
       </c>
       <c r="T59" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="U59" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="V59" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="W59" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="Y59" s="1" t="s">
         <v>40</v>
@@ -7899,10 +7897,10 @@
     </row>
     <row r="60" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>443</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>444</v>
       </c>
       <c r="C60" s="1" t="n">
         <v>2008</v>
@@ -7920,55 +7918,55 @@
         <v>1</v>
       </c>
       <c r="H60" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="I60" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="I60" s="1" t="s">
+      <c r="J60" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="J60" s="1" t="s">
+      <c r="K60" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="K60" s="1" t="s">
+      <c r="L60" s="6" t="s">
         <v>448</v>
       </c>
-      <c r="L60" s="6" t="s">
+      <c r="M60" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="M60" s="1" t="s">
+      <c r="N60" s="8" t="s">
         <v>450</v>
       </c>
-      <c r="N60" s="8" t="s">
+      <c r="O60" s="8" t="s">
         <v>451</v>
       </c>
-      <c r="O60" s="8" t="s">
+      <c r="P60" s="8" t="s">
         <v>452</v>
       </c>
-      <c r="P60" s="8" t="s">
+      <c r="Q60" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="Q60" s="1" t="s">
+      <c r="R60" s="5" t="s">
         <v>454</v>
-      </c>
-      <c r="R60" s="5" t="s">
-        <v>455</v>
       </c>
       <c r="S60" s="1" t="s">
         <v>62</v>
       </c>
       <c r="T60" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="U60" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="U60" s="1" t="s">
+      <c r="V60" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="V60" s="1" t="s">
+      <c r="W60" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="W60" s="1" t="s">
+      <c r="X60" s="1" t="s">
         <v>459</v>
-      </c>
-      <c r="X60" s="1" t="s">
-        <v>460</v>
       </c>
       <c r="Y60" s="1" t="s">
         <v>94</v>
@@ -7976,10 +7974,10 @@
     </row>
     <row r="61" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>461</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>462</v>
       </c>
       <c r="C61" s="1" t="n">
         <v>2011</v>
@@ -7994,55 +7992,55 @@
         <v>1</v>
       </c>
       <c r="H61" s="8" t="s">
+        <v>462</v>
+      </c>
+      <c r="I61" s="5" t="s">
         <v>463</v>
       </c>
-      <c r="I61" s="5" t="s">
+      <c r="J61" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="J61" s="1" t="s">
+      <c r="K61" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="K61" s="1" t="s">
+      <c r="L61" s="10" t="s">
         <v>466</v>
       </c>
-      <c r="L61" s="10" t="s">
+      <c r="M61" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="M61" s="1" t="s">
+      <c r="N61" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="N61" s="1" t="s">
+      <c r="O61" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="P61" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="O61" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="P61" s="1" t="s">
+      <c r="Q61" s="8" t="s">
         <v>470</v>
       </c>
-      <c r="Q61" s="8" t="s">
+      <c r="R61" s="5" t="s">
         <v>471</v>
-      </c>
-      <c r="R61" s="5" t="s">
-        <v>472</v>
       </c>
       <c r="S61" s="1" t="s">
         <v>34</v>
       </c>
       <c r="T61" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="U61" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="U61" s="1" t="s">
+      <c r="V61" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="V61" s="1" t="s">
+      <c r="W61" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="W61" s="1" t="s">
+      <c r="X61" s="1" t="s">
         <v>476</v>
-      </c>
-      <c r="X61" s="1" t="s">
-        <v>477</v>
       </c>
       <c r="Y61" s="1" t="s">
         <v>94</v>
@@ -8050,10 +8048,10 @@
     </row>
     <row r="62" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C62" s="1" t="n">
         <v>2011</v>
@@ -8080,7 +8078,7 @@
         <v>2</v>
       </c>
       <c r="L62" s="6" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M62" s="1" t="s">
         <v>78</v>
@@ -8107,16 +8105,16 @@
         <v>83</v>
       </c>
       <c r="U62" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="V62" s="1" t="s">
         <v>480</v>
-      </c>
-      <c r="V62" s="1" t="s">
-        <v>481</v>
       </c>
       <c r="W62" s="1" t="s">
         <v>38</v>
       </c>
       <c r="X62" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="Y62" s="1" t="s">
         <v>40</v>
@@ -8124,10 +8122,10 @@
     </row>
     <row r="63" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C63" s="1" t="n">
         <v>444444</v>
@@ -8142,13 +8140,13 @@
         <v>225</v>
       </c>
       <c r="T63" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="U63" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="U63" s="1" t="s">
+      <c r="V63" s="1" t="s">
         <v>485</v>
-      </c>
-      <c r="V63" s="1" t="s">
-        <v>486</v>
       </c>
       <c r="W63" s="1" t="s">
         <v>38</v>
@@ -8159,10 +8157,10 @@
     </row>
     <row r="64" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C64" s="1" t="n">
         <v>444444</v>
@@ -8177,13 +8175,13 @@
         <v>225</v>
       </c>
       <c r="T64" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="U64" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="V64" s="1" t="s">
         <v>488</v>
-      </c>
-      <c r="V64" s="1" t="s">
-        <v>489</v>
       </c>
       <c r="W64" s="1" t="s">
         <v>38</v>
@@ -8194,16 +8192,16 @@
     </row>
     <row r="65" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>490</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>491</v>
       </c>
       <c r="C65" s="1" t="n">
         <v>2011</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E65" s="1" t="n">
         <v>143</v>
@@ -8218,16 +8216,16 @@
         <v>15766</v>
       </c>
       <c r="I65" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="J65" s="1" t="s">
         <v>493</v>
-      </c>
-      <c r="J65" s="1" t="s">
-        <v>494</v>
       </c>
       <c r="K65" s="1" t="n">
         <v>2</v>
       </c>
       <c r="L65" s="11" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="M65" s="1" t="s">
         <v>324</v>
@@ -8245,7 +8243,7 @@
         <v>15766</v>
       </c>
       <c r="R65" s="5" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="S65" s="1" t="s">
         <v>34</v>
@@ -8254,10 +8252,10 @@
         <v>328</v>
       </c>
       <c r="U65" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="V65" s="1" t="s">
         <v>497</v>
-      </c>
-      <c r="V65" s="1" t="s">
-        <v>498</v>
       </c>
       <c r="W65" s="1" t="s">
         <v>38</v>
@@ -8268,10 +8266,10 @@
     </row>
     <row r="66" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C66" s="1" t="n">
         <v>2014</v>
@@ -8292,16 +8290,16 @@
         <v>20286</v>
       </c>
       <c r="I66" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="J66" s="1" t="s">
         <v>500</v>
-      </c>
-      <c r="J66" s="1" t="s">
-        <v>501</v>
       </c>
       <c r="K66" s="1" t="n">
         <v>2</v>
       </c>
       <c r="L66" s="6" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="M66" s="1" t="s">
         <v>324</v>
@@ -8319,7 +8317,7 @@
         <v>20286</v>
       </c>
       <c r="R66" s="5" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="S66" s="1" t="s">
         <v>34</v>
@@ -8328,10 +8326,10 @@
         <v>328</v>
       </c>
       <c r="U66" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="V66" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="W66" s="1" t="s">
         <v>38</v>
@@ -8342,10 +8340,10 @@
     </row>
     <row r="67" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>505</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>506</v>
       </c>
       <c r="C67" s="1" t="n">
         <v>444444</v>
@@ -8354,7 +8352,7 @@
         <v>150</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="G67" s="1" t="n">
         <v>1</v>
@@ -8363,28 +8361,28 @@
         <v>88</v>
       </c>
       <c r="Q67" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="R67" s="5" t="s">
         <v>508</v>
-      </c>
-      <c r="R67" s="5" t="s">
-        <v>509</v>
       </c>
       <c r="S67" s="1" t="s">
         <v>34</v>
       </c>
       <c r="T67" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="U67" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="U67" s="1" t="s">
+      <c r="V67" s="1" t="s">
         <v>511</v>
       </c>
-      <c r="V67" s="1" t="s">
+      <c r="W67" s="1" t="s">
         <v>512</v>
       </c>
-      <c r="W67" s="1" t="s">
+      <c r="X67" s="1" t="s">
         <v>513</v>
-      </c>
-      <c r="X67" s="1" t="s">
-        <v>514</v>
       </c>
       <c r="Y67" s="1" t="s">
         <v>40</v>
@@ -8392,16 +8390,16 @@
     </row>
     <row r="68" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C68" s="1" t="n">
         <v>2011</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E68" s="1" t="n">
         <v>149</v>
@@ -8419,7 +8417,7 @@
         <v>55</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="K68" s="1" t="n">
         <v>2</v>
@@ -8449,13 +8447,13 @@
         <v>34</v>
       </c>
       <c r="T68" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="U68" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="U68" s="1" t="s">
-        <v>511</v>
-      </c>
       <c r="V68" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="W68" s="1" t="s">
         <v>38</v>
@@ -8466,16 +8464,16 @@
     </row>
     <row r="69" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C69" s="1" t="n">
         <v>2014</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E69" s="1" t="n">
         <v>149</v>
@@ -8523,13 +8521,13 @@
         <v>34</v>
       </c>
       <c r="T69" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="U69" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="V69" s="1" t="s">
         <v>520</v>
-      </c>
-      <c r="U69" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="V69" s="1" t="s">
-        <v>521</v>
       </c>
       <c r="W69" s="1" t="s">
         <v>342</v>
@@ -8561,10 +8559,10 @@
         <v>88</v>
       </c>
       <c r="Q70" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="R70" s="5" t="s">
         <v>522</v>
-      </c>
-      <c r="R70" s="5" t="s">
-        <v>523</v>
       </c>
       <c r="S70" s="1" t="s">
         <v>34</v>
@@ -8573,16 +8571,16 @@
         <v>38</v>
       </c>
       <c r="U70" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="V70" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="V70" s="1" t="s">
+      <c r="W70" s="1" t="s">
         <v>525</v>
       </c>
-      <c r="W70" s="1" t="s">
+      <c r="X70" s="1" t="s">
         <v>526</v>
-      </c>
-      <c r="X70" s="1" t="s">
-        <v>527</v>
       </c>
       <c r="Y70" s="1" t="s">
         <v>40</v>
@@ -8593,16 +8591,16 @@
         <v>406</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C71" s="1" t="n">
         <v>444444</v>
       </c>
       <c r="E71" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="F71" s="1" t="s">
         <v>528</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>529</v>
       </c>
       <c r="G71" s="1" t="n">
         <v>1</v>
@@ -8611,10 +8609,10 @@
         <v>88</v>
       </c>
       <c r="Q71" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="R71" s="5" t="s">
         <v>530</v>
-      </c>
-      <c r="R71" s="5" t="s">
-        <v>531</v>
       </c>
       <c r="S71" s="1" t="s">
         <v>34</v>
@@ -8623,16 +8621,16 @@
         <v>38</v>
       </c>
       <c r="U71" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="V71" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="W71" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="W71" s="1" t="s">
+      <c r="X71" s="1" t="s">
         <v>533</v>
-      </c>
-      <c r="X71" s="1" t="s">
-        <v>534</v>
       </c>
       <c r="Y71" s="1" t="s">
         <v>40</v>
@@ -8640,10 +8638,10 @@
     </row>
     <row r="72" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C72" s="1" t="n">
         <v>444444</v>
@@ -8652,7 +8650,7 @@
         <v>147</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="G72" s="1" t="n">
         <v>1</v>
@@ -8664,10 +8662,10 @@
         <v>88</v>
       </c>
       <c r="Q72" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="R72" s="5" t="s">
         <v>537</v>
-      </c>
-      <c r="R72" s="5" t="s">
-        <v>538</v>
       </c>
       <c r="S72" s="1" t="s">
         <v>34</v>
@@ -8679,13 +8677,13 @@
         <v>370</v>
       </c>
       <c r="V72" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="W72" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="W72" s="1" t="s">
+      <c r="X72" s="1" t="s">
         <v>540</v>
-      </c>
-      <c r="X72" s="1" t="s">
-        <v>541</v>
       </c>
       <c r="Y72" s="1" t="s">
         <v>40</v>
@@ -8693,10 +8691,10 @@
     </row>
     <row r="73" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>542</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>543</v>
       </c>
       <c r="C73" s="1" t="n">
         <v>2009</v>
@@ -8735,7 +8733,7 @@
         <v>380</v>
       </c>
       <c r="P73" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="Q73" s="1" t="n">
         <v>18866</v>
@@ -8750,16 +8748,16 @@
         <v>383</v>
       </c>
       <c r="U73" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="V73" s="1" t="s">
         <v>545</v>
-      </c>
-      <c r="V73" s="1" t="s">
-        <v>546</v>
       </c>
       <c r="W73" s="1" t="s">
         <v>38</v>
       </c>
       <c r="X73" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="Y73" s="1" t="s">
         <v>94</v>
@@ -8767,10 +8765,10 @@
     </row>
     <row r="74" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C74" s="1" t="n">
         <v>2010</v>
@@ -8809,7 +8807,7 @@
         <v>380</v>
       </c>
       <c r="P74" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="Q74" s="1" t="n">
         <v>18866</v>
@@ -8824,16 +8822,16 @@
         <v>383</v>
       </c>
       <c r="U74" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="V74" s="1" t="s">
         <v>545</v>
-      </c>
-      <c r="V74" s="1" t="s">
-        <v>546</v>
       </c>
       <c r="W74" s="1" t="s">
         <v>38</v>
       </c>
       <c r="X74" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="Y74" s="1" t="s">
         <v>94</v>
@@ -8841,16 +8839,16 @@
     </row>
     <row r="75" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C75" s="1" t="n">
         <v>2011</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E75" s="1" t="n">
         <v>147</v>
@@ -8886,7 +8884,7 @@
         <v>380</v>
       </c>
       <c r="P75" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="Q75" s="1" t="n">
         <v>18866</v>
@@ -8901,16 +8899,16 @@
         <v>383</v>
       </c>
       <c r="U75" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="V75" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="W75" s="1" t="s">
         <v>38</v>
       </c>
       <c r="X75" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="Y75" s="1" t="s">
         <v>94</v>
@@ -8918,10 +8916,10 @@
     </row>
     <row r="76" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C76" s="1" t="n">
         <v>2012</v>
@@ -8960,7 +8958,7 @@
         <v>380</v>
       </c>
       <c r="P76" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="Q76" s="1" t="n">
         <v>18866</v>
@@ -8975,16 +8973,16 @@
         <v>383</v>
       </c>
       <c r="U76" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="V76" s="1" t="s">
         <v>545</v>
-      </c>
-      <c r="V76" s="1" t="s">
-        <v>546</v>
       </c>
       <c r="W76" s="1" t="s">
         <v>38</v>
       </c>
       <c r="X76" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="Y76" s="1" t="s">
         <v>94</v>
@@ -8992,10 +8990,10 @@
     </row>
     <row r="77" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C77" s="1" t="n">
         <v>2013</v>
@@ -9034,7 +9032,7 @@
         <v>380</v>
       </c>
       <c r="P77" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="Q77" s="1" t="n">
         <v>18866</v>
@@ -9049,16 +9047,16 @@
         <v>383</v>
       </c>
       <c r="U77" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="V77" s="1" t="s">
         <v>545</v>
-      </c>
-      <c r="V77" s="1" t="s">
-        <v>546</v>
       </c>
       <c r="W77" s="1" t="s">
         <v>38</v>
       </c>
       <c r="X77" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="Y77" s="1" t="s">
         <v>94</v>
@@ -9066,10 +9064,10 @@
     </row>
     <row r="78" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C78" s="1" t="n">
         <v>2014</v>
@@ -9111,7 +9109,7 @@
         <v>398</v>
       </c>
       <c r="P78" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="Q78" s="1" t="n">
         <v>21087</v>
@@ -9126,16 +9124,16 @@
         <v>383</v>
       </c>
       <c r="U78" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="V78" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="W78" s="1" t="s">
         <v>38</v>
       </c>
       <c r="X78" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="Y78" s="1" t="s">
         <v>94</v>
@@ -9143,10 +9141,10 @@
     </row>
     <row r="79" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>555</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>556</v>
       </c>
       <c r="C79" s="1" t="n">
         <v>2011</v>
@@ -9164,34 +9162,34 @@
         <v>14448</v>
       </c>
       <c r="I79" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="J79" s="1" t="s">
         <v>557</v>
-      </c>
-      <c r="J79" s="1" t="s">
-        <v>558</v>
       </c>
       <c r="K79" s="1" t="n">
         <v>2</v>
       </c>
       <c r="L79" s="11" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="M79" s="1" t="s">
         <v>153</v>
       </c>
       <c r="N79" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="O79" s="1" t="s">
         <v>155</v>
       </c>
       <c r="P79" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="Q79" s="1" t="s">
         <v>561</v>
       </c>
-      <c r="Q79" s="1" t="s">
+      <c r="R79" s="5" t="s">
         <v>562</v>
-      </c>
-      <c r="R79" s="5" t="s">
-        <v>563</v>
       </c>
       <c r="S79" s="1" t="s">
         <v>34</v>
@@ -9200,13 +9198,13 @@
         <v>158</v>
       </c>
       <c r="U79" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="V79" s="1" t="s">
         <v>564</v>
       </c>
-      <c r="V79" s="1" t="s">
+      <c r="W79" s="1" t="s">
         <v>565</v>
-      </c>
-      <c r="W79" s="1" t="s">
-        <v>566</v>
       </c>
       <c r="Y79" s="1" t="s">
         <v>40</v>
@@ -9214,10 +9212,10 @@
     </row>
     <row r="80" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>567</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>568</v>
       </c>
       <c r="C80" s="1" t="n">
         <v>2012</v>
@@ -9235,46 +9233,46 @@
         <v>16666</v>
       </c>
       <c r="I80" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="J80" s="1" t="s">
         <v>569</v>
-      </c>
-      <c r="J80" s="1" t="s">
-        <v>570</v>
       </c>
       <c r="K80" s="1" t="n">
         <v>2</v>
       </c>
       <c r="L80" s="6" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="M80" s="1" t="s">
         <v>153</v>
       </c>
       <c r="N80" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="O80" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="P80" s="1" t="s">
         <v>560</v>
-      </c>
-      <c r="O80" s="1" t="s">
-        <v>560</v>
-      </c>
-      <c r="P80" s="1" t="s">
-        <v>561</v>
       </c>
       <c r="Q80" s="1" t="n">
         <v>16666</v>
       </c>
       <c r="R80" s="5" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="S80" s="1" t="s">
         <v>34</v>
       </c>
       <c r="T80" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="U80" s="1" t="s">
         <v>573</v>
       </c>
-      <c r="U80" s="1" t="s">
+      <c r="V80" s="1" t="s">
         <v>574</v>
-      </c>
-      <c r="V80" s="1" t="s">
-        <v>575</v>
       </c>
       <c r="W80" s="1" t="s">
         <v>38</v>
@@ -9285,10 +9283,10 @@
     </row>
     <row r="81" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>576</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>577</v>
       </c>
       <c r="C81" s="1" t="n">
         <v>2017</v>
@@ -9315,7 +9313,7 @@
         <v>3</v>
       </c>
       <c r="L81" s="6" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="M81" s="1" t="s">
         <v>176</v>
@@ -9339,19 +9337,19 @@
         <v>34</v>
       </c>
       <c r="T81" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="U81" s="1" t="s">
         <v>579</v>
       </c>
-      <c r="U81" s="1" t="s">
+      <c r="V81" s="1" t="s">
         <v>580</v>
-      </c>
-      <c r="V81" s="1" t="s">
-        <v>581</v>
       </c>
       <c r="W81" s="1" t="s">
         <v>222</v>
       </c>
       <c r="X81" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="Y81" s="1" t="s">
         <v>94</v>
@@ -9359,10 +9357,10 @@
     </row>
     <row r="82" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>583</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>584</v>
       </c>
       <c r="C82" s="1" t="n">
         <v>2011</v>
@@ -9402,7 +9400,7 @@
         <v>155</v>
       </c>
       <c r="P82" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="Q82" s="1" t="n">
         <v>17086</v>
@@ -9414,19 +9412,19 @@
         <v>34</v>
       </c>
       <c r="T82" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="U82" s="1" t="s">
         <v>586</v>
       </c>
-      <c r="U82" s="1" t="s">
+      <c r="V82" s="1" t="s">
         <v>587</v>
-      </c>
-      <c r="V82" s="1" t="s">
-        <v>588</v>
       </c>
       <c r="W82" s="1" t="s">
         <v>38</v>
       </c>
       <c r="X82" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="Y82" s="1" t="s">
         <v>40</v>
@@ -9446,7 +9444,7 @@
         <v>150</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="G83" s="1" t="n">
         <v>1</v>
@@ -9458,10 +9456,10 @@
         <v>88</v>
       </c>
       <c r="Q83" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="R83" s="5" t="s">
         <v>591</v>
-      </c>
-      <c r="R83" s="5" t="s">
-        <v>592</v>
       </c>
       <c r="S83" s="1" t="s">
         <v>34</v>
@@ -9470,16 +9468,16 @@
         <v>38</v>
       </c>
       <c r="U83" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="V83" s="1" t="s">
         <v>593</v>
       </c>
-      <c r="V83" s="1" t="s">
+      <c r="W83" s="1" t="s">
         <v>594</v>
       </c>
-      <c r="W83" s="1" t="s">
+      <c r="X83" s="1" t="s">
         <v>595</v>
-      </c>
-      <c r="X83" s="1" t="s">
-        <v>596</v>
       </c>
       <c r="Y83" s="1" t="s">
         <v>40</v>
@@ -9523,13 +9521,13 @@
         <v>38</v>
       </c>
       <c r="U84" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="V84" s="1" t="s">
         <v>597</v>
       </c>
-      <c r="V84" s="1" t="s">
+      <c r="W84" s="1" t="s">
         <v>598</v>
-      </c>
-      <c r="W84" s="1" t="s">
-        <v>599</v>
       </c>
       <c r="Y84" s="1" t="s">
         <v>40</v>
@@ -9549,7 +9547,7 @@
         <v>150</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="G85" s="1" t="n">
         <v>1</v>
@@ -9561,10 +9559,10 @@
         <v>88</v>
       </c>
       <c r="Q85" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="R85" s="5" t="s">
         <v>591</v>
-      </c>
-      <c r="R85" s="5" t="s">
-        <v>592</v>
       </c>
       <c r="S85" s="1" t="s">
         <v>34</v>
@@ -9573,16 +9571,16 @@
         <v>38</v>
       </c>
       <c r="U85" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="V85" s="1" t="s">
         <v>600</v>
       </c>
-      <c r="V85" s="1" t="s">
+      <c r="W85" s="1" t="s">
         <v>601</v>
       </c>
-      <c r="W85" s="1" t="s">
+      <c r="X85" s="1" t="s">
         <v>602</v>
-      </c>
-      <c r="X85" s="1" t="s">
-        <v>603</v>
       </c>
       <c r="Y85" s="1" t="s">
         <v>40</v>
@@ -9590,10 +9588,10 @@
     </row>
     <row r="86" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C86" s="1" t="n">
         <v>2011</v>
@@ -9611,16 +9609,16 @@
         <v>14446</v>
       </c>
       <c r="I86" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="J86" s="1" t="s">
         <v>605</v>
-      </c>
-      <c r="J86" s="1" t="s">
-        <v>606</v>
       </c>
       <c r="K86" s="1" t="n">
         <v>7</v>
       </c>
       <c r="L86" s="6" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="M86" s="1" t="s">
         <v>153</v>
@@ -9632,31 +9630,31 @@
         <v>155</v>
       </c>
       <c r="P86" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="Q86" s="1" t="n">
         <v>14446</v>
       </c>
       <c r="R86" s="5" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="S86" s="1" t="s">
         <v>34</v>
       </c>
       <c r="T86" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="U86" s="1" t="s">
         <v>609</v>
       </c>
-      <c r="U86" s="1" t="s">
+      <c r="V86" s="1" t="s">
         <v>610</v>
-      </c>
-      <c r="V86" s="1" t="s">
-        <v>611</v>
       </c>
       <c r="W86" s="1" t="s">
         <v>38</v>
       </c>
       <c r="X86" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="Y86" s="1" t="s">
         <v>40</v>
@@ -9664,10 +9662,10 @@
     </row>
     <row r="87" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>613</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>614</v>
       </c>
       <c r="C87" s="1" t="n">
         <v>2008</v>
@@ -9685,19 +9683,19 @@
         <v>15086</v>
       </c>
       <c r="I87" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="J87" s="1" t="s">
         <v>615</v>
-      </c>
-      <c r="J87" s="1" t="s">
-        <v>616</v>
       </c>
       <c r="K87" s="1" t="n">
         <v>2</v>
       </c>
       <c r="L87" s="6" t="s">
+        <v>616</v>
+      </c>
+      <c r="M87" s="1" t="s">
         <v>617</v>
-      </c>
-      <c r="M87" s="1" t="s">
-        <v>618</v>
       </c>
       <c r="N87" s="1" t="s">
         <v>177</v>
@@ -9706,31 +9704,31 @@
         <v>177</v>
       </c>
       <c r="P87" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="Q87" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="Q87" s="1" t="s">
+      <c r="R87" s="5" t="s">
         <v>620</v>
-      </c>
-      <c r="R87" s="5" t="s">
-        <v>621</v>
       </c>
       <c r="S87" s="1" t="s">
         <v>62</v>
       </c>
       <c r="T87" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="U87" s="1" t="s">
         <v>622</v>
       </c>
-      <c r="U87" s="1" t="s">
+      <c r="V87" s="1" t="s">
         <v>623</v>
       </c>
-      <c r="V87" s="1" t="s">
+      <c r="W87" s="1" t="s">
         <v>624</v>
       </c>
-      <c r="W87" s="1" t="s">
+      <c r="X87" s="1" t="s">
         <v>625</v>
-      </c>
-      <c r="X87" s="1" t="s">
-        <v>626</v>
       </c>
       <c r="Y87" s="1" t="s">
         <v>94</v>
@@ -9738,10 +9736,10 @@
     </row>
     <row r="88" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C88" s="1" t="n">
         <v>2011</v>
@@ -9795,13 +9793,13 @@
         <v>34</v>
       </c>
       <c r="T88" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="U88" s="1" t="s">
         <v>628</v>
       </c>
-      <c r="U88" s="1" t="s">
+      <c r="V88" s="1" t="s">
         <v>629</v>
-      </c>
-      <c r="V88" s="1" t="s">
-        <v>630</v>
       </c>
       <c r="W88" s="1" t="s">
         <v>38</v>
@@ -9812,10 +9810,10 @@
     </row>
     <row r="89" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C89" s="1" t="n">
         <v>2011</v>
@@ -9872,10 +9870,10 @@
         <v>83</v>
       </c>
       <c r="U89" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="V89" s="1" t="s">
         <v>632</v>
-      </c>
-      <c r="V89" s="1" t="s">
-        <v>633</v>
       </c>
       <c r="W89" s="1" t="s">
         <v>38</v>
@@ -9886,24 +9884,24 @@
     </row>
     <row r="90" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="13" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="H90" s="12" t="n">
         <v>27266</v>
       </c>
       <c r="I90" s="12" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="R90" s="14"/>
     </row>
     <row r="91" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="12" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="R91" s="14"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:X91"/>
+  <autoFilter ref="A1:X89"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -9926,7 +9924,7 @@
       <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.30859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="15" width="19.28"/>
@@ -9935,33 +9933,33 @@
   <sheetData>
     <row r="1" s="16" customFormat="true" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
+        <v>636</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>637</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="C1" s="16" t="s">
         <v>638</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>639</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>640</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
+        <v>641</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>642</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="15" t="s">
         <v>643</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="D2" s="15" t="s">
         <v>644</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>645</v>
       </c>
       <c r="E2" s="8" t="n">
         <v>0</v>
@@ -9969,16 +9967,16 @@
     </row>
     <row r="3" customFormat="false" ht="35.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
+        <v>645</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>643</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>646</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>643</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>644</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>647</v>
       </c>
       <c r="E3" s="8" t="n">
         <v>0</v>
@@ -9986,16 +9984,16 @@
     </row>
     <row r="4" customFormat="false" ht="69.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
+        <v>647</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>648</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" s="15" t="s">
         <v>649</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="D4" s="15" t="s">
         <v>650</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>651</v>
       </c>
       <c r="E4" s="8" t="n">
         <v>0</v>
@@ -10003,16 +10001,16 @@
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
+        <v>651</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>652</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>643</v>
-      </c>
-      <c r="C5" s="15" t="s">
+      <c r="D5" s="15" t="s">
         <v>653</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>654</v>
       </c>
       <c r="E5" s="8" t="n">
         <v>0</v>
@@ -10020,16 +10018,16 @@
     </row>
     <row r="6" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
+        <v>654</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>655</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C6" s="15" t="s">
         <v>656</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="D6" s="15" t="s">
         <v>657</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>658</v>
       </c>
       <c r="E6" s="8" t="n">
         <v>0</v>
@@ -10037,16 +10035,16 @@
     </row>
     <row r="7" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
+        <v>658</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>659</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>643</v>
-      </c>
-      <c r="C7" s="15" t="s">
+      <c r="D7" s="15" t="s">
         <v>660</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>661</v>
       </c>
       <c r="E7" s="8" t="n">
         <v>0</v>
@@ -10054,16 +10052,16 @@
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
+        <v>661</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>655</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>662</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>656</v>
-      </c>
-      <c r="C8" s="15" t="s">
+      <c r="D8" s="15" t="s">
         <v>663</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>664</v>
       </c>
       <c r="E8" s="8" t="n">
         <v>0</v>
@@ -10071,16 +10069,16 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
+        <v>664</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>655</v>
+      </c>
+      <c r="C9" s="15" t="s">
         <v>665</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>656</v>
-      </c>
-      <c r="C9" s="15" t="s">
+      <c r="D9" s="15" t="s">
         <v>666</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>667</v>
       </c>
       <c r="E9" s="8" t="n">
         <v>0</v>
@@ -10088,16 +10086,16 @@
     </row>
     <row r="10" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
+        <v>667</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>652</v>
+      </c>
+      <c r="D10" s="15" t="s">
         <v>668</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>643</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>653</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>669</v>
       </c>
       <c r="E10" s="8" t="n">
         <v>0</v>
@@ -10105,16 +10103,16 @@
     </row>
     <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
+        <v>669</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="C11" s="15" t="s">
         <v>670</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>643</v>
-      </c>
-      <c r="C11" s="15" t="s">
+      <c r="D11" s="15" t="s">
         <v>671</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>672</v>
       </c>
       <c r="E11" s="8" t="n">
         <v>0</v>
@@ -10125,13 +10123,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="C12" s="15" t="s">
+        <v>672</v>
+      </c>
+      <c r="D12" s="15" t="s">
         <v>673</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>674</v>
       </c>
       <c r="E12" s="8" t="n">
         <v>0</v>
@@ -10142,13 +10140,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="8" t="s">
+        <v>674</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>670</v>
+      </c>
+      <c r="D13" s="15" t="s">
         <v>675</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>671</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>676</v>
       </c>
       <c r="E13" s="8" t="n">
         <v>0</v>
@@ -10156,16 +10154,16 @@
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
+        <v>676</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>677</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>643</v>
-      </c>
-      <c r="C14" s="15" t="s">
+      <c r="D14" s="15" t="s">
         <v>678</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>679</v>
       </c>
       <c r="E14" s="8" t="n">
         <v>0</v>
@@ -10176,13 +10174,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C15" s="15" t="s">
+        <v>679</v>
+      </c>
+      <c r="D15" s="15" t="s">
         <v>680</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>681</v>
       </c>
       <c r="E15" s="8" t="n">
         <v>0</v>
@@ -10190,16 +10188,16 @@
     </row>
     <row r="16" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
+        <v>681</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="C16" s="15" t="s">
         <v>682</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>643</v>
-      </c>
-      <c r="C16" s="15" t="s">
+      <c r="D16" s="15" t="s">
         <v>683</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>684</v>
       </c>
       <c r="E16" s="8" t="n">
         <v>0</v>
@@ -10207,16 +10205,16 @@
     </row>
     <row r="17" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
+        <v>684</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>685</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>643</v>
-      </c>
-      <c r="C17" s="8" t="s">
+      <c r="D17" s="15" t="s">
         <v>686</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>687</v>
       </c>
       <c r="E17" s="8" t="n">
         <v>0</v>
@@ -10227,13 +10225,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C18" s="8" t="s">
+        <v>687</v>
+      </c>
+      <c r="D18" s="15" t="s">
         <v>688</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>689</v>
       </c>
       <c r="E18" s="8" t="n">
         <v>0</v>
@@ -10244,13 +10242,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C19" s="0" t="s">
+        <v>689</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>690</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>691</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>0</v>
@@ -10258,16 +10256,16 @@
     </row>
     <row r="20" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C20" s="15" t="s">
+        <v>691</v>
+      </c>
+      <c r="D20" s="15" t="s">
         <v>692</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>693</v>
       </c>
       <c r="E20" s="8" t="n">
         <v>0</v>
@@ -10275,16 +10273,16 @@
     </row>
     <row r="21" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C21" s="15" t="s">
+        <v>693</v>
+      </c>
+      <c r="D21" s="15" t="s">
         <v>694</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>695</v>
       </c>
       <c r="E21" s="8" t="n">
         <v>0</v>
@@ -10292,16 +10290,16 @@
     </row>
     <row r="22" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
+        <v>695</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="C22" s="15" t="s">
         <v>696</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>643</v>
-      </c>
-      <c r="C22" s="15" t="s">
+      <c r="D22" s="15" t="s">
         <v>697</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>698</v>
       </c>
       <c r="E22" s="8" t="n">
         <v>0</v>
@@ -10309,16 +10307,16 @@
     </row>
     <row r="23" customFormat="false" ht="35.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="E23" s="8" t="n">
         <v>0</v>
@@ -10326,16 +10324,16 @@
     </row>
     <row r="24" customFormat="false" ht="35.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="s">
+        <v>699</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>652</v>
+      </c>
+      <c r="D24" s="15" t="s">
         <v>700</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>643</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>653</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>701</v>
       </c>
       <c r="E24" s="8" t="n">
         <v>0</v>
@@ -10343,16 +10341,16 @@
     </row>
     <row r="25" customFormat="false" ht="35.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="s">
+        <v>701</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>652</v>
+      </c>
+      <c r="D25" s="15" t="s">
         <v>702</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>643</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>653</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>703</v>
       </c>
       <c r="E25" s="8" t="n">
         <v>0</v>
@@ -10363,13 +10361,13 @@
         <v>24</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E26" s="8" t="n">
         <v>0</v>

</xml_diff>